<commit_message>
add get domain config api for toolkit portal
</commit_message>
<xml_diff>
--- a/workflow/project_info.xlsx
+++ b/workflow/project_info.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA8AEFF-4EE3-4BA7-BA88-590AE450CAC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0B142B-C08B-4882-BAB3-B499DA61B746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Java-Api" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="210">
   <si>
     <t>Project Name</t>
   </si>
@@ -911,6 +911,33 @@
   </si>
   <si>
     <t>EnableCloudRoamingHandler : ICloudNotificationHandler</t>
+  </si>
+  <si>
+    <t>https://toolkit.helix-playground.net/api/v1</t>
+  </si>
+  <si>
+    <t>/guest/config</t>
+  </si>
+  <si>
+    <t>get domain config</t>
+  </si>
+  <si>
+    <t>REACT_APP_GAME_ASSET_URL</t>
+  </si>
+  <si>
+    <t>operatorSettings.service</t>
+  </si>
+  <si>
+    <t>central-games-management-web</t>
+  </si>
+  <si>
+    <t>QuickReloadController</t>
+  </si>
+  <si>
+    <t>GuestPortalAdminController</t>
+  </si>
+  <si>
+    <t>quick reload</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1049,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1068,6 +1095,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,7 +1212,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1267,6 +1300,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1386,6 +1428,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1863,44 +1911,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:J19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.7109375" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="12" t="s">
@@ -1963,370 +2011,406 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B5" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27" t="s">
+      <c r="C5" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E5" s="72" t="s">
         <v>176</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27" t="s">
+      <c r="F5" s="72" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H5" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="I5" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J5" s="35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A5" s="35" t="s">
+    <row r="6" spans="1:10" ht="14.45" customHeight="1">
+      <c r="A6" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B6" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C6" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>124</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="J5" s="33"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="14" t="s">
-        <v>125</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>118</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="33"/>
+        <v>154</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
       <c r="D7" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>118</v>
       </c>
       <c r="F7" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="36"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="33"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="14" t="s">
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="36"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F9" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="33"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="14" t="s">
         <v>124</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="33"/>
+        <v>156</v>
+      </c>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="35" t="s">
-        <v>119</v>
-      </c>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
       <c r="D11" s="14" t="s">
         <v>124</v>
       </c>
       <c r="E11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="36"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
       <c r="D12" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>119</v>
       </c>
       <c r="F12" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="J12" s="36"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="35" t="s">
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D14" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E14" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F14" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="35" t="s">
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="14" t="s">
+      <c r="J14" s="36"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F15" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="14" t="s">
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="36"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F16" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="33"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="35" t="s">
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="36"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D17" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="35" t="s">
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="J16" s="33"/>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="22" t="s">
+      <c r="J17" s="36"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E18" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F18" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="33"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="14" t="s">
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="36"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D19" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="33"/>
-    </row>
-    <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="23" t="s">
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="36"/>
+    </row>
+    <row r="20" spans="1:10" ht="30">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D20" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E20" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F20" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="34"/>
-    </row>
-    <row r="20" spans="1:10" customFormat="1"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="37"/>
+    </row>
     <row r="21" spans="1:10" customFormat="1"/>
     <row r="22" spans="1:10" customFormat="1"/>
     <row r="23" spans="1:10" customFormat="1"/>
     <row r="24" spans="1:10" customFormat="1"/>
     <row r="25" spans="1:10" customFormat="1"/>
     <row r="26" spans="1:10" customFormat="1"/>
-    <row r="30" spans="1:10">
-      <c r="B30"/>
-    </row>
+    <row r="27" spans="1:10" customFormat="1"/>
     <row r="31" spans="1:10">
       <c r="B31"/>
     </row>
     <row r="32" spans="1:10">
       <c r="B32"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="J4:J19"/>
-    <mergeCell ref="A5:A19"/>
-    <mergeCell ref="G5:G19"/>
-    <mergeCell ref="I5:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="H5:H19"/>
-    <mergeCell ref="C5:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B5:B19"/>
+    <mergeCell ref="J5:J20"/>
+    <mergeCell ref="A6:A20"/>
+    <mergeCell ref="G6:G20"/>
+    <mergeCell ref="I6:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="H6:H20"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B6:B20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{5B40A53B-4297-4647-BE1D-8AAF8F0A3AF4}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{1B5D53D2-B7A7-4B0C-9EFB-101FC5ED7B36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2334,7 +2418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -2353,21 +2437,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="F1" s="43"/>
+      <c r="G1" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="12" t="s">
@@ -2399,10 +2483,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.9" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>191</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2411,7 +2495,7 @@
       <c r="D3" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="42" t="s">
         <v>147</v>
       </c>
       <c r="F3" s="14" t="s">
@@ -2423,20 +2507,20 @@
       <c r="H3" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="42" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="14" t="s">
         <v>152</v>
       </c>
@@ -2446,18 +2530,18 @@
       <c r="H4" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="42"/>
       <c r="F5" s="14" t="s">
         <v>151</v>
       </c>
@@ -2467,13 +2551,13 @@
       <c r="H5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="39"/>
+      <c r="I5" s="42"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="48" t="s">
         <v>194</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -2482,7 +2566,7 @@
       <c r="D6" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="44" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="27" t="s">
@@ -2499,15 +2583,15 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="27" t="s">
         <v>124</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="E7" s="41"/>
+      <c r="E7" s="44"/>
       <c r="F7" s="27" t="s">
         <v>188</v>
       </c>
@@ -2522,15 +2606,15 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
       <c r="C8" s="27" t="s">
         <v>124</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="E8" s="41"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="27" t="s">
         <v>189</v>
       </c>
@@ -2539,15 +2623,15 @@
       <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="27" t="s">
         <v>125</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="41"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="27" t="s">
         <v>190</v>
       </c>
@@ -2628,16 +2712,16 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="53" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -2648,10 +2732,10 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="55"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="7" t="s">
         <v>59</v>
       </c>
@@ -2660,10 +2744,10 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="55"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2672,14 +2756,14 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="55"/>
-      <c r="B6" s="49" t="s">
+      <c r="A6" s="58"/>
+      <c r="B6" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="54" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -2690,10 +2774,10 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="55"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
@@ -2702,10 +2786,10 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="55"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="A8" s="58"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2714,12 +2798,12 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="55"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="51" t="s">
+      <c r="A9" s="58"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="54" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -2730,10 +2814,10 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="55"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="A10" s="58"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
       <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
@@ -2742,10 +2826,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="60">
-      <c r="A11" s="55"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
+      <c r="A11" s="58"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
       <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
@@ -2754,10 +2838,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="60">
-      <c r="A12" s="56"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
@@ -2766,14 +2850,14 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49" t="s">
+      <c r="B13" s="52"/>
+      <c r="C13" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="52" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -2784,10 +2868,10 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="47"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
@@ -2796,10 +2880,10 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
@@ -2808,10 +2892,10 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="47"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="51" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="54" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2822,10 +2906,10 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="47"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="52"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2834,10 +2918,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="47"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="52"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="3" t="s">
         <v>23</v>
       </c>
@@ -2846,10 +2930,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="60">
-      <c r="A19" s="47"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="52"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="3" t="s">
         <v>25</v>
       </c>
@@ -2858,10 +2942,10 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="52"/>
+      <c r="A20" s="50"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
@@ -2870,10 +2954,10 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="47"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="53"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="56"/>
       <c r="E21" s="3" t="s">
         <v>27</v>
       </c>
@@ -2882,8 +2966,8 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="47"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="52"/>
       <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
@@ -2898,8 +2982,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="75">
-      <c r="A23" s="47"/>
-      <c r="B23" s="60" t="s">
+      <c r="A23" s="50"/>
+      <c r="B23" s="63" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -2916,15 +3000,15 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="47"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="60" t="s">
+      <c r="A24" s="50"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="60" t="s">
         <v>36</v>
       </c>
       <c r="F24" s="7" t="s">
@@ -2932,31 +3016,31 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="47"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="58"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="61"/>
       <c r="F25" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="47"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="59"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="47"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="63" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="66" t="s">
         <v>35</v>
       </c>
       <c r="F27" s="7" t="s">
@@ -2964,22 +3048,22 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="47"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="64"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="67"/>
       <c r="F28" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="47"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="60" t="s">
+      <c r="A29" s="50"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="60" t="s">
+      <c r="D29" s="63" t="s">
         <v>37</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -2990,10 +3074,10 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="47"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="62"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="7" t="s">
         <v>59</v>
       </c>
@@ -3002,10 +3086,10 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="47"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="60" t="s">
+      <c r="A31" s="50"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="63" t="s">
         <v>39</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -3016,10 +3100,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="30">
-      <c r="A32" s="48"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
+      <c r="A32" s="51"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="7" t="s">
         <v>59</v>
       </c>
@@ -3065,7 +3149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -3107,7 +3191,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2"/>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="68" t="s">
         <v>83</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -3122,7 +3206,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2"/>
-      <c r="B4" s="65"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="16"/>
       <c r="D4" s="18" t="s">
         <v>72</v>
@@ -3133,7 +3217,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2"/>
-      <c r="B5" s="65"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="16"/>
       <c r="D5" s="18"/>
       <c r="E5" s="17" t="s">
@@ -3142,7 +3226,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2"/>
-      <c r="B6" s="65"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="16"/>
       <c r="D6" s="18"/>
       <c r="E6" s="17" t="s">
@@ -3151,7 +3235,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2"/>
-      <c r="B7" s="65"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="17" t="s">
@@ -3160,7 +3244,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2"/>
-      <c r="B8" s="65"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="17" t="s">
@@ -3169,7 +3253,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2"/>
-      <c r="B9" s="65"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="17" t="s">
@@ -3178,7 +3262,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2"/>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="68" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -3191,11 +3275,11 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65" t="s">
+      <c r="B11" s="68"/>
+      <c r="C11" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="69" t="s">
         <v>60</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -3204,38 +3288,38 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="67"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="67"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65" t="s">
+      <c r="B15" s="68"/>
+      <c r="C15" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="66" t="s">
+      <c r="D15" s="69" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="18" t="s">
@@ -3244,34 +3328,34 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="67"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="70"/>
       <c r="E16" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="67"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="70"/>
       <c r="E17" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="68" t="s">
         <v>83</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -3286,7 +3370,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2"/>
-      <c r="B20" s="65"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="16" t="s">
         <v>88</v>
       </c>
@@ -3299,7 +3383,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2"/>
-      <c r="B21" s="65"/>
+      <c r="B21" s="68"/>
       <c r="C21" t="s">
         <v>199</v>
       </c>

</xml_diff>

<commit_message>
add enable cloud roaming
</commit_message>
<xml_diff>
--- a/workflow/project_info.xlsx
+++ b/workflow/project_info.xlsx
@@ -3,23 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0B142B-C08B-4882-BAB3-B499DA61B746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91844F16-1341-4073-809D-AE849E8BCF55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Java-Api" sheetId="4" r:id="rId1"/>
-    <sheet name="Python-Api" sheetId="5" r:id="rId2"/>
-    <sheet name="Cloud2StoresWF" sheetId="1" r:id="rId3"/>
-    <sheet name="toolkitNotify" sheetId="2" r:id="rId4"/>
-    <sheet name="EnableBalanceSyncRoam" sheetId="3" r:id="rId5"/>
+    <sheet name="01-Java-Api" sheetId="4" r:id="rId1"/>
+    <sheet name="02-Python-Api" sheetId="5" r:id="rId2"/>
+    <sheet name="03-Store2StoresWF" sheetId="1" r:id="rId3"/>
+    <sheet name="04-ToolkitNotify" sheetId="2" r:id="rId4"/>
+    <sheet name="05-EnableCloudRoaming" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId6"/>
+    <sheet name="EnableBalanceSyncRoam" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="233">
   <si>
     <t>Project Name</t>
   </si>
@@ -898,9 +900,6 @@
     <t>GuestBalanceOneTimePullEndpoint</t>
   </si>
   <si>
-    <t>OneTimeBalancePullTask.cs</t>
-  </si>
-  <si>
     <t>CreateLocationBalanceSyncQueueEndpoint</t>
   </si>
   <si>
@@ -938,13 +937,85 @@
   </si>
   <si>
     <t>quick reload</t>
+  </si>
+  <si>
+    <t>Locaction Type</t>
+  </si>
+  <si>
+    <t>IsStore</t>
+  </si>
+  <si>
+    <t>IsHeadOffice</t>
+  </si>
+  <si>
+    <t>IsCentralReportLocation</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>autoupdate.service</t>
+  </si>
+  <si>
+    <t>add variable "Enable Guest Balance Push At UTC"</t>
+  </si>
+  <si>
+    <t>UploadCardBalance</t>
+  </si>
+  <si>
+    <t>Handler</t>
+  </si>
+  <si>
+    <t>OneTimeGuestBalancePushTask (Reason == InitialBalance &amp;&amp; g.SentAt == null)</t>
+  </si>
+  <si>
+    <t>OneTimeCardBalanceAndStatePullTask.cs</t>
+  </si>
+  <si>
+    <t>GetCardsForOperatorByLocationId</t>
+  </si>
+  <si>
+    <t>/api/v1/api/v1/card</t>
+  </si>
+  <si>
+    <t>api/v1/card/location{location-id}</t>
+  </si>
+  <si>
+    <t>Add Variable</t>
+  </si>
+  <si>
+    <t>Push Task in Store</t>
+  </si>
+  <si>
+    <t>Push Api on Cloud</t>
+  </si>
+  <si>
+    <t>Pull Api on Could</t>
+  </si>
+  <si>
+    <t>OneTimeCardBalanceAndStatePullTask</t>
+  </si>
+  <si>
+    <t>update_balance_pull_status</t>
+  </si>
+  <si>
+    <t>Update Balance pull status</t>
+  </si>
+  <si>
+    <t>send_enable_cloud_roaming_notification</t>
+  </si>
+  <si>
+    <t>_update_ho_global_cards_type</t>
+  </si>
+  <si>
+    <t>DisableGlobalCardsTask</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1047,6 +1118,12 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1212,7 +1289,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1309,6 +1386,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1339,26 +1422,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1393,30 +1500,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1429,11 +1512,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1913,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1933,22 +2016,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="12" t="s">
@@ -2013,73 +2096,73 @@
     <row r="4" spans="1:10">
       <c r="A4" s="30"/>
       <c r="B4" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>124</v>
       </c>
       <c r="E4" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="F4" s="30" t="s">
         <v>202</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>203</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>181</v>
       </c>
       <c r="H4" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="I4" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="J4" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="J4" s="29" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="72" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="72" t="s">
-        <v>207</v>
-      </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="F5" s="72" t="s">
-        <v>209</v>
-      </c>
-      <c r="G5" s="72" t="s">
+      <c r="F5" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="H5" s="72" t="s">
+      <c r="H5" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="72" t="s">
+      <c r="I5" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="J5" s="35" t="s">
+      <c r="J5" s="37" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.45" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="40" t="s">
         <v>118</v>
       </c>
       <c r="D6" s="14" t="s">
@@ -2091,21 +2174,21 @@
       <c r="F6" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="36"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="14" t="s">
         <v>125</v>
       </c>
@@ -2115,15 +2198,15 @@
       <c r="F7" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="36"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="38"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="14" t="s">
         <v>126</v>
       </c>
@@ -2133,15 +2216,15 @@
       <c r="F8" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="36"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="38"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
       <c r="D9" s="14" t="s">
         <v>127</v>
       </c>
@@ -2151,15 +2234,15 @@
       <c r="F9" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="36"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="14" t="s">
         <v>124</v>
       </c>
@@ -2169,15 +2252,15 @@
       <c r="F10" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="36"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="42"/>
       <c r="D11" s="14" t="s">
         <v>124</v>
       </c>
@@ -2187,15 +2270,15 @@
       <c r="F11" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="36"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="38" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="40" t="s">
         <v>119</v>
       </c>
       <c r="D12" s="14" t="s">
@@ -2207,17 +2290,17 @@
       <c r="F12" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="38" t="s">
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="J12" s="36"/>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="14" t="s">
         <v>126</v>
       </c>
@@ -2227,15 +2310,15 @@
       <c r="F13" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="36"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="38" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="40" t="s">
         <v>120</v>
       </c>
       <c r="D14" s="22" t="s">
@@ -2247,17 +2330,17 @@
       <c r="F14" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="38" t="s">
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="J14" s="36"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
       <c r="D15" s="14" t="s">
         <v>126</v>
       </c>
@@ -2267,15 +2350,15 @@
       <c r="F15" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="36"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
       <c r="D16" s="14" t="s">
         <v>125</v>
       </c>
@@ -2285,15 +2368,15 @@
       <c r="F16" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="36"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="39"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="38" t="s">
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="40" t="s">
         <v>121</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -2305,17 +2388,17 @@
       <c r="F17" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="38" t="s">
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="J17" s="36"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="22" t="s">
         <v>125</v>
       </c>
@@ -2325,14 +2408,14 @@
       <c r="F18" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="36"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="14" t="s">
         <v>122</v>
       </c>
@@ -2345,14 +2428,14 @@
       <c r="F19" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="36"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="23" t="s">
         <v>123</v>
       </c>
@@ -2365,10 +2448,10 @@
       <c r="F20" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
       <c r="I20" s="14"/>
-      <c r="J20" s="37"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10" customFormat="1"/>
     <row r="22" spans="1:10" customFormat="1"/>
@@ -2419,7 +2502,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2437,21 +2520,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43" t="s">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="12" t="s">
@@ -2483,10 +2566,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.9" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="49" t="s">
         <v>191</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2495,7 +2578,7 @@
       <c r="D3" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="49" t="s">
         <v>147</v>
       </c>
       <c r="F3" s="14" t="s">
@@ -2507,20 +2590,20 @@
       <c r="H3" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="49" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="42"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="14" t="s">
         <v>152</v>
       </c>
@@ -2530,18 +2613,18 @@
       <c r="H4" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="I4" s="42"/>
+      <c r="I4" s="49"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="42"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="14" t="s">
         <v>124</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="42"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="14" t="s">
         <v>151</v>
       </c>
@@ -2551,7 +2634,7 @@
       <c r="H5" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="42"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="45" t="s">
@@ -2599,7 +2682,7 @@
         <v>195</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="I7" s="27" t="s">
         <v>83</v>
@@ -2636,10 +2719,10 @@
         <v>190</v>
       </c>
       <c r="G9" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>197</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>198</v>
       </c>
       <c r="I9" s="27" t="s">
         <v>83</v>
@@ -2657,16 +2740,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2681,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2712,16 +2795,16 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="63" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -2732,10 +2815,10 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="58"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="7" t="s">
         <v>59</v>
       </c>
@@ -2744,10 +2827,10 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="58"/>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
+      <c r="A5" s="68"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2756,14 +2839,14 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="58"/>
-      <c r="B6" s="52" t="s">
+      <c r="A6" s="68"/>
+      <c r="B6" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="64" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -2774,10 +2857,10 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="58"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
+      <c r="A7" s="68"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
@@ -2786,10 +2869,10 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="58"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
       <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
@@ -2798,12 +2881,12 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="58"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="54" t="s">
+      <c r="A9" s="68"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -2814,10 +2897,10 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="58"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
       <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
@@ -2826,10 +2909,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="60">
-      <c r="A11" s="58"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
       <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
@@ -2838,10 +2921,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="60">
-      <c r="A12" s="59"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
       <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
@@ -2850,28 +2933,28 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52" t="s">
+      <c r="B13" s="62"/>
+      <c r="C13" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="62" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="50"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
       <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
@@ -2880,10 +2963,10 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="50"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
       <c r="E15" s="3" t="s">
         <v>50</v>
       </c>
@@ -2892,10 +2975,10 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="50"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="54" t="s">
+      <c r="A16" s="60"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="64" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -2906,10 +2989,10 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="50"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="55"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2918,10 +3001,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30">
-      <c r="A18" s="50"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="55"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="65"/>
       <c r="E18" s="3" t="s">
         <v>23</v>
       </c>
@@ -2930,10 +3013,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="60">
-      <c r="A19" s="50"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="55"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="65"/>
       <c r="E19" s="3" t="s">
         <v>25</v>
       </c>
@@ -2942,10 +3025,10 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="50"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="55"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="65"/>
       <c r="E20" s="3" t="s">
         <v>28</v>
       </c>
@@ -2954,10 +3037,10 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="50"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="56"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="66"/>
       <c r="E21" s="3" t="s">
         <v>27</v>
       </c>
@@ -2966,8 +3049,8 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="50"/>
-      <c r="B22" s="52"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="62"/>
       <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
@@ -2982,8 +3065,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="75">
-      <c r="A23" s="50"/>
-      <c r="B23" s="63" t="s">
+      <c r="A23" s="60"/>
+      <c r="B23" s="54" t="s">
         <v>48</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -3000,15 +3083,15 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="50"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="63" t="s">
+      <c r="A24" s="60"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="51" t="s">
         <v>36</v>
       </c>
       <c r="F24" s="7" t="s">
@@ -3016,31 +3099,31 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="50"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="61"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="52"/>
       <c r="F25" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="50"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="62"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="53"/>
       <c r="F26" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="50"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="66" t="s">
+      <c r="A27" s="60"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="57" t="s">
         <v>35</v>
       </c>
       <c r="F27" s="7" t="s">
@@ -3048,22 +3131,22 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="50"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="67"/>
+      <c r="A28" s="60"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="50"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="63" t="s">
+      <c r="A29" s="60"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="63" t="s">
+      <c r="D29" s="54" t="s">
         <v>37</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -3074,10 +3157,10 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="50"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
+      <c r="A30" s="60"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="56"/>
       <c r="E30" s="7" t="s">
         <v>59</v>
       </c>
@@ -3086,10 +3169,10 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="50"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="63" t="s">
+      <c r="A31" s="60"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="54" t="s">
         <v>39</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -3100,10 +3183,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="30">
-      <c r="A32" s="51"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="65"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
       <c r="E32" s="7" t="s">
         <v>59</v>
       </c>
@@ -3113,14 +3196,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D24:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E27:E28"/>
     <mergeCell ref="A13:A32"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="C16:C21"/>
@@ -3135,6 +3210,14 @@
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="A3:A12"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3191,7 +3274,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2"/>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="70" t="s">
         <v>83</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -3206,7 +3289,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2"/>
-      <c r="B4" s="68"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="16"/>
       <c r="D4" s="18" t="s">
         <v>72</v>
@@ -3217,7 +3300,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2"/>
-      <c r="B5" s="68"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="16"/>
       <c r="D5" s="18"/>
       <c r="E5" s="17" t="s">
@@ -3226,7 +3309,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2"/>
-      <c r="B6" s="68"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="16"/>
       <c r="D6" s="18"/>
       <c r="E6" s="17" t="s">
@@ -3235,7 +3318,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2"/>
-      <c r="B7" s="68"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
       <c r="E7" s="17" t="s">
@@ -3244,7 +3327,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2"/>
-      <c r="B8" s="68"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
       <c r="E8" s="17" t="s">
@@ -3253,7 +3336,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2"/>
-      <c r="B9" s="68"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="17" t="s">
@@ -3262,7 +3345,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2"/>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="70" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="18" t="s">
@@ -3275,11 +3358,11 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68" t="s">
+      <c r="B11" s="70"/>
+      <c r="C11" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="71" t="s">
         <v>60</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -3288,38 +3371,38 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="70"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="71"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68" t="s">
+      <c r="B15" s="70"/>
+      <c r="C15" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="71" t="s">
         <v>61</v>
       </c>
       <c r="E15" s="18" t="s">
@@ -3328,34 +3411,34 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="70"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="18" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="70"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="68"/>
-      <c r="D18" s="71"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="70" t="s">
         <v>83</v>
       </c>
       <c r="C19" s="16" t="s">
@@ -3370,7 +3453,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2"/>
-      <c r="B20" s="68"/>
+      <c r="B20" s="70"/>
       <c r="C20" s="16" t="s">
         <v>88</v>
       </c>
@@ -3383,12 +3466,12 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2"/>
-      <c r="B21" s="68"/>
+      <c r="B21" s="70"/>
       <c r="C21" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="28" t="s">
         <v>199</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>200</v>
       </c>
       <c r="E21" s="28" t="s">
         <v>99</v>
@@ -3450,6 +3533,169 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7636E11A-DD37-4E2A-9C82-5FDE6B1C11EE}">
+  <dimension ref="B1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="D1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
+        <v>229</v>
+      </c>
+      <c r="F13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="75" t="s">
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" display="https://card-balance-api.helix-playground.net/api/v1/api/v1/card" xr:uid="{DD08568C-9837-4EC0-BC49-147755C0A08B}"/>
+    <hyperlink ref="D11" r:id="rId2" display="https://card-balance-api.helix-playground.net/api/v1/api/v1/card/location{location-id}" xr:uid="{D2FBFFA6-DD77-4A31-AAC6-5C671B6EB03F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC40E2A-8B8A-40E0-94FA-7EC1ADE5A1DF}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1"/>
   <sheetViews>

</xml_diff>